<commit_message>
updating MSCI_AC_WORLD and STOXX50 folder
</commit_message>
<xml_diff>
--- a/MSCI_AC_WORLD/MSCIACW_with_donuts.xlsx
+++ b/MSCI_AC_WORLD/MSCIACW_with_donuts.xlsx
@@ -1,38 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c060ac0a7f9c7ae2/main/DELL_NB/EU/MSCI_AC_WORLD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_65023BFC96051B16865B01188F1D806E015EFE98" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04F9B00A-AB34-44BB-89D0-7C2FB7DBE5B7}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="38280" yWindow="480" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="全球权重" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="欧洲权重" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="全球权重" sheetId="1" r:id="rId1"/>
+    <sheet name="欧洲权重" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>国家</t>
+  </si>
+  <si>
+    <t>权重（%）</t>
+  </si>
+  <si>
+    <t>美国</t>
+  </si>
+  <si>
+    <t>欧洲</t>
+  </si>
+  <si>
+    <t>日本</t>
+  </si>
+  <si>
+    <t>中国</t>
+  </si>
+  <si>
+    <t>加拿大</t>
+  </si>
+  <si>
+    <t>其他国家</t>
+  </si>
+  <si>
+    <t>英国</t>
+  </si>
+  <si>
+    <t>法国</t>
+  </si>
+  <si>
+    <t>瑞士</t>
+  </si>
+  <si>
+    <t>德国</t>
+  </si>
+  <si>
+    <t>荷兰</t>
+  </si>
+  <si>
+    <t>其他欧洲国家</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,124 +114,86 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>3</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="44796075" cy="22679025"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>6774</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="11068049" cy="5603450"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495425" y="578274"/>
+          <a:ext cx="11068049" cy="5603450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,180 +480,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>国家</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>权重（%）</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>美国</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>65.75</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>欧洲</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>16.8</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>日本</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>4.71</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>中国</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>3.01</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>加拿大</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>2.71</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>其他国家</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>6.02</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>国家</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>权重（%）</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>英国</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>3.27</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>法国</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
         <v>2.73</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>瑞士</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2.47</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>德国</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
         <v>2.31</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>荷兰</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1.11</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>其他欧洲国家</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
         <v>4.91</v>
       </c>
     </row>

</xml_diff>